<commit_message>
feat: Implement cricket format selection and overs calculation fix
- Added format selection feature allowing users to choose between T20, ODI, First Class, or custom formats.
- Introduced CRICKET_FORMATS dictionary in models.py to define format specifications.
- Updated input_handlers.py to include select_format() for interactive format selection.
- Refactored main.py to integrate format selection into the match flow.
- Enhanced innings logic in game_logic.py to accommodate unlimited overs and bowler limits based on selected format.
- Fixed overs calculation in models.py to use bowler_overs as the authoritative source, resolving discrepancies in displayed overs.
- Created comprehensive tests for format configuration and overs calculation accuracy.
- Added documentation for new features and fixes in the docs/ directory.
</commit_message>
<xml_diff>
--- a/scorecard_generator/exports/scorecard.xlsx
+++ b/scorecard_generator/exports/scorecard.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,14 +431,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>England: 12/0</t>
+          <t>England: 18/0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Match tied!</t>
+          <t>England win by 10 wicket(s)!</t>
         </is>
       </c>
     </row>
@@ -867,7 +867,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jos Buttler</t>
+          <t>Chris Jordan</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -992,20 +992,20 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>600.00</t>
         </is>
       </c>
     </row>
@@ -1021,10 +1021,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -1361,19 +1361,19 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Adam Zampa</t>
+          <t>Josh Hazlewood</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1385,48 +1385,12 @@
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Josh Hazlewood</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
-        <v>6</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>